<commit_message>
add roundOf prices in analyzes module
</commit_message>
<xml_diff>
--- a/helix.xlsx
+++ b/helix.xlsx
@@ -9864,9 +9864,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9874,6 +9871,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -10172,14 +10172,14 @@
   <dimension ref="A1:C1577"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A851" workbookViewId="0">
-      <selection activeCell="E854" sqref="E854"/>
+      <selection activeCell="C851" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -10189,16 +10189,16 @@
       <c r="B1" s="1" t="s">
         <v>3240</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3241</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -10487,11 +10487,11 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
@@ -10659,11 +10659,11 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" ht="24">
       <c r="A46" s="2" t="s">
@@ -12910,11 +12910,11 @@
       </c>
     </row>
     <row r="250" spans="1:3">
-      <c r="A250" s="5" t="s">
+      <c r="A250" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="B250" s="5"/>
-      <c r="C250" s="7"/>
+      <c r="B250" s="8"/>
+      <c r="C250" s="6"/>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="2" t="s">
@@ -14226,11 +14226,11 @@
       </c>
     </row>
     <row r="370" spans="1:3">
-      <c r="A370" s="5" t="s">
+      <c r="A370" s="8" t="s">
         <v>781</v>
       </c>
-      <c r="B370" s="5"/>
-      <c r="C370" s="7"/>
+      <c r="B370" s="8"/>
+      <c r="C370" s="6"/>
     </row>
     <row r="371" spans="1:3" ht="24">
       <c r="A371" s="2" t="s">
@@ -15080,11 +15080,11 @@
       </c>
     </row>
     <row r="448" spans="1:3">
-      <c r="A448" s="5" t="s">
+      <c r="A448" s="8" t="s">
         <v>944</v>
       </c>
-      <c r="B448" s="5"/>
-      <c r="C448" s="7"/>
+      <c r="B448" s="8"/>
+      <c r="C448" s="6"/>
     </row>
     <row r="449" spans="1:3" ht="24">
       <c r="A449" s="2" t="s">
@@ -15945,11 +15945,11 @@
       </c>
     </row>
     <row r="527" spans="1:3">
-      <c r="A527" s="5" t="s">
+      <c r="A527" s="8" t="s">
         <v>1105</v>
       </c>
-      <c r="B527" s="5"/>
-      <c r="C527" s="7"/>
+      <c r="B527" s="8"/>
+      <c r="C527" s="6"/>
     </row>
     <row r="528" spans="1:3" ht="24">
       <c r="A528" s="2" t="s">
@@ -16502,11 +16502,11 @@
       </c>
     </row>
     <row r="578" spans="1:3">
-      <c r="A578" s="5" t="s">
+      <c r="A578" s="8" t="s">
         <v>1207</v>
       </c>
-      <c r="B578" s="5"/>
-      <c r="C578" s="7"/>
+      <c r="B578" s="8"/>
+      <c r="C578" s="6"/>
     </row>
     <row r="579" spans="1:3" ht="60">
       <c r="A579" s="2" t="s">
@@ -16927,11 +16927,11 @@
       </c>
     </row>
     <row r="617" spans="1:3">
-      <c r="A617" s="5" t="s">
+      <c r="A617" s="8" t="s">
         <v>1299</v>
       </c>
-      <c r="B617" s="5"/>
-      <c r="C617" s="7"/>
+      <c r="B617" s="8"/>
+      <c r="C617" s="6"/>
     </row>
     <row r="618" spans="1:3" ht="24">
       <c r="A618" s="2" t="s">
@@ -18144,11 +18144,11 @@
       </c>
     </row>
     <row r="728" spans="1:3">
-      <c r="A728" s="5" t="s">
+      <c r="A728" s="8" t="s">
         <v>1531</v>
       </c>
-      <c r="B728" s="5"/>
-      <c r="C728" s="7"/>
+      <c r="B728" s="8"/>
+      <c r="C728" s="6"/>
     </row>
     <row r="729" spans="1:3">
       <c r="A729" s="2" t="s">
@@ -18470,11 +18470,11 @@
       </c>
     </row>
     <row r="758" spans="1:3">
-      <c r="A758" s="5" t="s">
+      <c r="A758" s="8" t="s">
         <v>1591</v>
       </c>
-      <c r="B758" s="5"/>
-      <c r="C758" s="7"/>
+      <c r="B758" s="8"/>
+      <c r="C758" s="6"/>
     </row>
     <row r="759" spans="1:3" ht="60">
       <c r="A759" s="2" t="s">
@@ -18488,11 +18488,11 @@
       </c>
     </row>
     <row r="760" spans="1:3">
-      <c r="A760" s="5" t="s">
+      <c r="A760" s="8" t="s">
         <v>1595</v>
       </c>
-      <c r="B760" s="5"/>
-      <c r="C760" s="7"/>
+      <c r="B760" s="8"/>
+      <c r="C760" s="6"/>
     </row>
     <row r="761" spans="1:3" ht="24">
       <c r="A761" s="2" t="s">
@@ -18583,11 +18583,11 @@
       </c>
     </row>
     <row r="769" spans="1:3">
-      <c r="A769" s="5" t="s">
+      <c r="A769" s="8" t="s">
         <v>1616</v>
       </c>
-      <c r="B769" s="5"/>
-      <c r="C769" s="7"/>
+      <c r="B769" s="8"/>
+      <c r="C769" s="6"/>
     </row>
     <row r="770" spans="1:3" ht="48">
       <c r="A770" s="2" t="s">
@@ -19448,11 +19448,11 @@
       </c>
     </row>
     <row r="848" spans="1:3">
-      <c r="A848" s="5" t="s">
+      <c r="A848" s="8" t="s">
         <v>1775</v>
       </c>
-      <c r="B848" s="5"/>
-      <c r="C848" s="7"/>
+      <c r="B848" s="8"/>
+      <c r="C848" s="6"/>
     </row>
     <row r="849" spans="1:3" ht="60">
       <c r="A849" s="2" t="s">
@@ -19532,11 +19532,11 @@
       </c>
     </row>
     <row r="856" spans="1:3">
-      <c r="A856" s="5" t="s">
+      <c r="A856" s="8" t="s">
         <v>1791</v>
       </c>
-      <c r="B856" s="5"/>
-      <c r="C856" s="7"/>
+      <c r="B856" s="8"/>
+      <c r="C856" s="6"/>
     </row>
     <row r="857" spans="1:3" ht="24">
       <c r="A857" s="2" t="s">
@@ -19671,11 +19671,11 @@
       </c>
     </row>
     <row r="869" spans="1:3">
-      <c r="A869" s="5" t="s">
+      <c r="A869" s="8" t="s">
         <v>1820</v>
       </c>
-      <c r="B869" s="5"/>
-      <c r="C869" s="7"/>
+      <c r="B869" s="8"/>
+      <c r="C869" s="6"/>
     </row>
     <row r="870" spans="1:3" ht="60">
       <c r="A870" s="2" t="s">
@@ -24309,11 +24309,11 @@
       </c>
     </row>
     <row r="1291" spans="1:3">
-      <c r="A1291" s="5" t="s">
+      <c r="A1291" s="8" t="s">
         <v>2667</v>
       </c>
-      <c r="B1291" s="5"/>
-      <c r="C1291" s="7"/>
+      <c r="B1291" s="8"/>
+      <c r="C1291" s="6"/>
     </row>
     <row r="1292" spans="1:3">
       <c r="A1292" s="2" t="s">
@@ -25933,11 +25933,11 @@
       </c>
     </row>
     <row r="1439" spans="1:3">
-      <c r="A1439" s="5" t="s">
+      <c r="A1439" s="8" t="s">
         <v>3025</v>
       </c>
-      <c r="B1439" s="5"/>
-      <c r="C1439" s="7"/>
+      <c r="B1439" s="8"/>
+      <c r="C1439" s="6"/>
     </row>
     <row r="1440" spans="1:3">
       <c r="A1440" s="2" t="s">
@@ -26028,11 +26028,11 @@
       </c>
     </row>
     <row r="1448" spans="1:3">
-      <c r="A1448" s="5" t="s">
+      <c r="A1448" s="8" t="s">
         <v>3042</v>
       </c>
-      <c r="B1448" s="5"/>
-      <c r="C1448" s="7"/>
+      <c r="B1448" s="8"/>
+      <c r="C1448" s="6"/>
     </row>
     <row r="1449" spans="1:3" ht="36">
       <c r="A1449" s="2" t="s">
@@ -26365,11 +26365,11 @@
       </c>
     </row>
     <row r="1479" spans="1:3">
-      <c r="A1479" s="5" t="s">
+      <c r="A1479" s="8" t="s">
         <v>3110</v>
       </c>
-      <c r="B1479" s="5"/>
-      <c r="C1479" s="7"/>
+      <c r="B1479" s="8"/>
+      <c r="C1479" s="6"/>
     </row>
     <row r="1480" spans="1:3">
       <c r="A1480" s="2" t="s">
@@ -26427,11 +26427,11 @@
       </c>
     </row>
     <row r="1485" spans="1:3">
-      <c r="A1485" s="5" t="s">
+      <c r="A1485" s="8" t="s">
         <v>3242</v>
       </c>
-      <c r="B1485" s="5"/>
-      <c r="C1485" s="7"/>
+      <c r="B1485" s="8"/>
+      <c r="C1485" s="6"/>
     </row>
     <row r="1486" spans="1:3">
       <c r="A1486" s="2" t="s">
@@ -26445,11 +26445,11 @@
       </c>
     </row>
     <row r="1487" spans="1:3">
-      <c r="A1487" s="5" t="s">
+      <c r="A1487" s="8" t="s">
         <v>3124</v>
       </c>
-      <c r="B1487" s="5"/>
-      <c r="C1487" s="7"/>
+      <c r="B1487" s="8"/>
+      <c r="C1487" s="6"/>
     </row>
     <row r="1488" spans="1:3" ht="24">
       <c r="A1488" s="2" t="s">
@@ -27443,16 +27443,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A728:B728"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A250:B250"/>
-    <mergeCell ref="A370:B370"/>
-    <mergeCell ref="A448:B448"/>
-    <mergeCell ref="A527:B527"/>
-    <mergeCell ref="A578:B578"/>
-    <mergeCell ref="A617:B617"/>
     <mergeCell ref="A1487:B1487"/>
     <mergeCell ref="A758:B758"/>
     <mergeCell ref="A760:B760"/>
@@ -27465,6 +27455,16 @@
     <mergeCell ref="A1448:B1448"/>
     <mergeCell ref="A1479:B1479"/>
     <mergeCell ref="A1485:B1485"/>
+    <mergeCell ref="A728:B728"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A250:B250"/>
+    <mergeCell ref="A370:B370"/>
+    <mergeCell ref="A448:B448"/>
+    <mergeCell ref="A527:B527"/>
+    <mergeCell ref="A578:B578"/>
+    <mergeCell ref="A617:B617"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>